<commit_message>
Gestione pagine multiple | richiesta regione
</commit_message>
<xml_diff>
--- a/aziende.xlsx
+++ b/aziende.xlsx
@@ -25,45 +25,45 @@
     <t>sito</t>
   </si>
   <si>
+    <t>Fattoria il Casalone</t>
+  </si>
+  <si>
+    <t>Azienda Agricola Barbialla Srl Società Agricola - Castello di Barbialla</t>
+  </si>
+  <si>
+    <t>Elleci Riviera</t>
+  </si>
+  <si>
+    <t>Azienda Agricola Ulivelli</t>
+  </si>
+  <si>
+    <t>Fattoria Ruschi Noceti</t>
+  </si>
+  <si>
+    <t>Saniscope-Chimica</t>
+  </si>
+  <si>
+    <t>Frantoio Carmignani Umberto</t>
+  </si>
+  <si>
+    <t>Castello di Gabbiano</t>
+  </si>
+  <si>
+    <t>Tenute Silvio Nardi</t>
+  </si>
+  <si>
+    <t>Rocca di Castagnoli Società Agricola</t>
+  </si>
+  <si>
+    <t>Archa</t>
+  </si>
+  <si>
+    <t>Ortofrutta Branchi</t>
+  </si>
+  <si>
     <t>Fattoria San Leolino</t>
   </si>
   <si>
-    <t>Azienda Agricola Barbialla Srl Società Agricola - Castello di Barbialla</t>
-  </si>
-  <si>
-    <t>Elleci Riviera</t>
-  </si>
-  <si>
-    <t>Fattoria il Casalone</t>
-  </si>
-  <si>
-    <t>Azienda Agricola Ulivelli</t>
-  </si>
-  <si>
-    <t>Fattoria Ruschi Noceti</t>
-  </si>
-  <si>
-    <t>Saniscope-Chimica</t>
-  </si>
-  <si>
-    <t>Frantoio Carmignani Umberto</t>
-  </si>
-  <si>
-    <t>Castello di Gabbiano</t>
-  </si>
-  <si>
-    <t>Tenute Silvio Nardi</t>
-  </si>
-  <si>
-    <t>Rocca di Castagnoli Società Agricola</t>
-  </si>
-  <si>
-    <t>Archa</t>
-  </si>
-  <si>
-    <t>Ortofrutta Branchi</t>
-  </si>
-  <si>
     <t>Azienda Agricola Magnani Gigliola</t>
   </si>
   <si>
@@ -100,40 +100,40 @@
     <t>Blitz Service</t>
   </si>
   <si>
+    <t>http://www.agriturismocasalone.com</t>
+  </si>
+  <si>
+    <t>https://www.aziendaagricolabarbialla.it</t>
+  </si>
+  <si>
+    <t>https://elleciriviera.it/</t>
+  </si>
+  <si>
+    <t>http://www.agricolaulivelli.it</t>
+  </si>
+  <si>
+    <t>http://www.fattoriaruschinoceti.com</t>
+  </si>
+  <si>
+    <t>http://www.saniscope-chimica.it/</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>http://www.castellogabbiano.it</t>
+  </si>
+  <si>
+    <t>https://www.tenutenardi.com/</t>
+  </si>
+  <si>
+    <t>https://www.roccadicastagnoli.com/</t>
+  </si>
+  <si>
+    <t>https://www.archa.it/</t>
+  </si>
+  <si>
     <t>http://www.fattoriasanleolino.com</t>
-  </si>
-  <si>
-    <t>https://www.aziendaagricolabarbialla.it</t>
-  </si>
-  <si>
-    <t>https://elleciriviera.it/</t>
-  </si>
-  <si>
-    <t>http://www.agriturismocasalone.com</t>
-  </si>
-  <si>
-    <t>http://www.agricolaulivelli.it</t>
-  </si>
-  <si>
-    <t>http://www.fattoriaruschinoceti.com</t>
-  </si>
-  <si>
-    <t>http://www.saniscope-chimica.it/</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>http://www.castellogabbiano.it</t>
-  </si>
-  <si>
-    <t>https://www.tenutenardi.com/</t>
-  </si>
-  <si>
-    <t>https://www.roccadicastagnoli.com/</t>
-  </si>
-  <si>
-    <t>https://www.archa.it/</t>
   </si>
   <si>
     <t>https://www.aziendagricolamagnanigigliola.com</t>
@@ -607,7 +607,7 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -615,7 +615,7 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -647,16 +647,16 @@
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>38</v>
+      <c r="B13" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
-        <v>34</v>
+      <c r="B14" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -672,7 +672,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -688,7 +688,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -712,7 +712,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -764,11 +764,11 @@
     <hyperlink ref="B5" r:id="rId4"/>
     <hyperlink ref="B6" r:id="rId5"/>
     <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId7"/>
     <hyperlink ref="B10" r:id="rId8"/>
     <hyperlink ref="B11" r:id="rId9"/>
     <hyperlink ref="B12" r:id="rId10"/>
-    <hyperlink ref="B13" r:id="rId11"/>
+    <hyperlink ref="B14" r:id="rId11"/>
     <hyperlink ref="B15" r:id="rId12"/>
     <hyperlink ref="B17" r:id="rId13"/>
     <hyperlink ref="B19" r:id="rId14"/>

</xml_diff>